<commit_message>
adding VI table to spreadsheet
</commit_message>
<xml_diff>
--- a/general_files_backup/reu_hours.xlsx
+++ b/general_files_backup/reu_hours.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dusty\Documents\REU_2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dusty\Documents\REU_2024\mtech_reu_plants\general_files_backup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AFCAFAF-C0A7-49A9-9FB7-769631D0F26C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{527280D8-E90D-4858-9E8F-9806211B6698}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D452F573-9CCD-483D-BC75-6E9E83E63D52}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="1" xr2:uid="{D452F573-9CCD-483D-BC75-6E9E83E63D52}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="VI table" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>date</t>
   </si>
@@ -51,6 +52,51 @@
   </si>
   <si>
     <t>weekly</t>
+  </si>
+  <si>
+    <t>Vegetation Indices</t>
+  </si>
+  <si>
+    <t>Index Name</t>
+  </si>
+  <si>
+    <t>Abbreviation</t>
+  </si>
+  <si>
+    <t>Equation</t>
+  </si>
+  <si>
+    <t>ExG</t>
+  </si>
+  <si>
+    <t>ExR</t>
+  </si>
+  <si>
+    <t>ExG-ExR</t>
+  </si>
+  <si>
+    <t>GRVI</t>
+  </si>
+  <si>
+    <t>RGBVI</t>
+  </si>
+  <si>
+    <t>Excess Red</t>
+  </si>
+  <si>
+    <t>Excess Green</t>
+  </si>
+  <si>
+    <t>Green Red Vegetation Index</t>
+  </si>
+  <si>
+    <t>Red Green Blue Vegetation Index</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>Bendig et al., 2015</t>
   </si>
 </sst>
 </file>
@@ -425,7 +471,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{484B4E20-0AD1-4A6D-A9A7-C7C2C32ECB23}">
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+    <sheetView topLeftCell="A38" workbookViewId="0">
       <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
@@ -1000,4 +1046,86 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B96BEEC9-6459-482D-BA08-B4DEA918BFF7}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>